<commit_message>
working on budget justification
</commit_message>
<xml_diff>
--- a/docs/proposals/NSF/budgets/budgetFSU.xlsx
+++ b/docs/proposals/NSF/budgets/budgetFSU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bquaife/projects/erosion/docs/proposals/NSF/budgets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2440E1-7DBA-2B47-9115-7521B3DD6CE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C887891D-17AC-8A4A-B791-4889962EEB03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="2260" windowWidth="26320" windowHeight="25500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="520" windowWidth="26320" windowHeight="25500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="budg 1" sheetId="4" r:id="rId1"/>
@@ -888,7 +888,7 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -989,19 +989,19 @@
       </c>
       <c r="C6" s="4">
         <f>C5*$I$18</f>
-        <v>1800.2876279384618</v>
+        <v>1956.4673283692312</v>
       </c>
       <c r="D6" s="4">
         <f>D5*$I$18</f>
-        <v>1854.2962567766156</v>
+        <v>2015.1613482203081</v>
       </c>
       <c r="E6" s="4">
         <f>E5*$I$18</f>
-        <v>954.93981220000001</v>
+        <v>1037.7833598000002</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" ref="F6" si="0">SUM(C6:E6)</f>
-        <v>4609.5236969150774</v>
+        <v>5009.4120363895399</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>10</v>
@@ -1049,19 +1049,19 @@
       </c>
       <c r="C8" s="4">
         <f>(C7*$I$11) + ($I$5*$I$10)</f>
-        <v>1986</v>
+        <v>2091</v>
       </c>
       <c r="D8" s="4">
         <f>(D7*$I$11) + ($I$5*$I$10)</f>
-        <v>1986.63</v>
+        <v>2094.7800000000002</v>
       </c>
       <c r="E8" s="4">
         <f>(E7*$I$11) + ($I$5*$I$10)</f>
-        <v>1987.2789</v>
+        <v>2098.6734000000001</v>
       </c>
       <c r="F8" s="4">
         <f>SUM(C8:E8)</f>
-        <v>5959.9089000000004</v>
+        <v>6284.4534000000003</v>
       </c>
       <c r="H8" s="15" t="s">
         <v>12</v>
@@ -1118,25 +1118,25 @@
       </c>
       <c r="C11" s="4">
         <f t="shared" si="1"/>
-        <v>3786.2876279384618</v>
+        <v>4047.4673283692309</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>3840.9262567766154</v>
+        <v>4109.9413482203081</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="1"/>
-        <v>2942.2187122</v>
+        <v>3136.4567598000003</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" ref="F11:F12" si="2" xml:space="preserve"> SUM(C11:E11)</f>
-        <v>10569.432596915078</v>
+        <v>11293.86543638954</v>
       </c>
       <c r="H11" s="18" t="s">
         <v>15</v>
       </c>
       <c r="I11" s="19">
-        <v>1E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1146,19 +1146,19 @@
       <c r="B12" s="1"/>
       <c r="C12" s="3">
         <f>C10+C11</f>
-        <v>35338.970089476919</v>
+        <v>35600.149789907693</v>
       </c>
       <c r="D12" s="3">
         <f>D10+D11</f>
-        <v>36340.189192161233</v>
+        <v>36609.204283604922</v>
       </c>
       <c r="E12" s="3">
         <f>E10+E11</f>
-        <v>30818.655712200001</v>
+        <v>31012.893759800001</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="2"/>
-        <v>102497.81499383817</v>
+        <v>103222.24783331262</v>
       </c>
       <c r="H12" s="18" t="s">
         <v>16</v>
@@ -1278,10 +1278,10 @@
         <v>28</v>
       </c>
       <c r="I18" s="19">
-        <v>0.1706</v>
+        <v>0.18540000000000001</v>
       </c>
       <c r="J18" s="26">
-        <v>0.1706</v>
+        <v>0.18540000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -1395,19 +1395,19 @@
       </c>
       <c r="C23" s="3">
         <f>C20+C12+C21+C22</f>
-        <v>44174.870089476921</v>
+        <v>44436.049789907695</v>
       </c>
       <c r="D23" s="3">
         <f>D20+D12+D21+D22</f>
-        <v>45749.448192161231</v>
+        <v>46018.46328360492</v>
       </c>
       <c r="E23" s="3">
         <f>E20+E12+E21+E22</f>
-        <v>40302.155712200001</v>
+        <v>40496.393759800005</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="4"/>
-        <v>130226.47399383815</v>
+        <v>130950.90683331262</v>
       </c>
       <c r="H23" s="24" t="s">
         <v>45</v>
@@ -1422,19 +1422,19 @@
       </c>
       <c r="C24" s="3">
         <f>C20+C12</f>
-        <v>36838.970089476919</v>
+        <v>37100.149789907693</v>
       </c>
       <c r="D24" s="3">
         <f>D20+D12</f>
-        <v>38340.189192161233</v>
+        <v>38609.204283604922</v>
       </c>
       <c r="E24" s="3">
         <f>E20+E12</f>
-        <v>32818.655712200001</v>
+        <v>33012.893759800005</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="4"/>
-        <v>107997.81499383817</v>
+        <v>108722.24783331262</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1455,19 +1455,19 @@
       </c>
       <c r="C26" s="3">
         <f>C24*$I$21</f>
-        <v>19893.043848317539</v>
+        <v>20034.080886550157</v>
       </c>
       <c r="D26" s="3">
         <f>D24*$I$21</f>
-        <v>20703.702163767066</v>
+        <v>20848.970313146659</v>
       </c>
       <c r="E26" s="3">
         <f>E24*$I$21</f>
-        <v>17722.074084588003</v>
+        <v>17826.962630292004</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="4"/>
-        <v>58318.820096672614</v>
+        <v>58710.01382998882</v>
       </c>
       <c r="H26" s="39"/>
       <c r="I26" s="39"/>
@@ -1479,19 +1479,19 @@
       <c r="B27"/>
       <c r="C27" s="3">
         <f>C23+C26</f>
-        <v>64067.913937794459</v>
+        <v>64470.130676457848</v>
       </c>
       <c r="D27" s="3">
         <f>D23+D26</f>
-        <v>66453.150355928301</v>
+        <v>66867.43359675158</v>
       </c>
       <c r="E27" s="3">
         <f>E23+E26</f>
-        <v>58024.229796788</v>
+        <v>58323.356390092013</v>
       </c>
       <c r="F27" s="27">
         <f t="shared" si="4"/>
-        <v>188545.29409051075</v>
+        <v>189660.92066330143</v>
       </c>
       <c r="H27" s="40"/>
       <c r="I27" s="40"/>

</xml_diff>